<commit_message>
update before pres to Martina
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CB47B3-726A-4913-A40B-3164D69D4E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B39E24-7080-461A-B14F-7609AAF44397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="111">
   <si>
     <t>Region</t>
   </si>
@@ -364,10 +364,13 @@
     <t>Westwood Lake</t>
   </si>
   <si>
-    <t>Pend d'Oreille</t>
-  </si>
-  <si>
     <t>Kootenay-Boundary</t>
+  </si>
+  <si>
+    <t>Pend-d'Oreille River</t>
+  </si>
+  <si>
+    <t>Current Projects / 3rd Party Interest (1 to 3)</t>
   </si>
 </sst>
 </file>
@@ -751,7 +754,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,6 +762,7 @@
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -771,7 +775,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -783,6 +789,9 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -794,6 +803,9 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -805,6 +817,9 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -816,6 +831,9 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -827,16 +845,22 @@
       <c r="C6" t="s">
         <v>107</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
         <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -901,7 +925,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed asian clam vars
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B39E24-7080-461A-B14F-7609AAF44397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790F59A-0DC6-4C38-8130-B5AF22FDB44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="2" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -753,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6445779-2465-4917-922C-4EA6D80CF35A}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9ABB0D-65E2-4F7D-8309-D592BA9BA411}">
   <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,10 +1197,10 @@
         <v>44</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1236,22 +1236,22 @@
         <v>1</v>
       </c>
       <c r="O4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="b">
         <v>1</v>
       </c>
       <c r="T4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="b">
         <v>1</v>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="W4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Added field for native species in wb
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790F59A-0DC6-4C38-8130-B5AF22FDB44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B40079C-BB80-4BEF-8902-D8AE38CB6AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="2" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6445779-2465-4917-922C-4EA6D80CF35A}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,11 +937,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9ABB0D-65E2-4F7D-8309-D592BA9BA411}">
   <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Add waterbody area in square kilometers
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B40079C-BB80-4BEF-8902-D8AE38CB6AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19E406E-4084-4245-834A-78E8EBC7A084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="110">
   <si>
     <t>Region</t>
   </si>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t>Pend-d'Oreille River</t>
-  </si>
-  <si>
-    <t>Current Projects / 3rd Party Interest (1 to 3)</t>
   </si>
 </sst>
 </file>
@@ -753,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6445779-2465-4917-922C-4EA6D80CF35A}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,9 +772,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -789,9 +784,6 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -803,9 +795,6 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -817,9 +806,6 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -831,9 +817,6 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -845,9 +828,6 @@
       <c r="C6" t="s">
         <v>107</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -858,9 +838,6 @@
       </c>
       <c r="C7" t="s">
         <v>109</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -937,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9ABB0D-65E2-4F7D-8309-D592BA9BA411}">
   <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -1055,13 +1032,13 @@
         <v>1</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -1129,7 +1106,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1138,13 +1115,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
@@ -1212,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -1221,13 +1198,13 @@
         <v>1</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
@@ -1295,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -1304,13 +1281,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" t="b">
         <v>1</v>
@@ -1378,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -1387,13 +1364,13 @@
         <v>1</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
@@ -1461,7 +1438,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -1470,13 +1447,13 @@
         <v>1</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
@@ -1544,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1553,13 +1530,13 @@
         <v>1</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="b">
         <v>1</v>
@@ -1627,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -1636,13 +1613,13 @@
         <v>1</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
@@ -1710,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -1719,13 +1696,13 @@
         <v>1</v>
       </c>
       <c r="I10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
@@ -1793,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1802,13 +1779,13 @@
         <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" t="b">
         <v>1</v>
@@ -1876,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1885,13 +1862,13 @@
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="b">
         <v>1</v>
@@ -1959,7 +1936,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1968,13 +1945,13 @@
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" t="b">
         <v>1</v>
@@ -2042,7 +2019,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -2051,13 +2028,13 @@
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" t="b">
         <v>1</v>
@@ -2125,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -2134,13 +2111,13 @@
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" t="b">
         <v>1</v>
@@ -2208,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -2217,13 +2194,13 @@
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
@@ -2291,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -2300,13 +2277,13 @@
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
@@ -2374,7 +2351,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -2383,13 +2360,13 @@
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" t="b">
         <v>1</v>
@@ -2457,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -2466,13 +2443,13 @@
         <v>1</v>
       </c>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" t="b">
         <v>1</v>
@@ -2540,7 +2517,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -2549,13 +2526,13 @@
         <v>1</v>
       </c>
       <c r="I20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
@@ -2623,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -2632,13 +2609,13 @@
         <v>1</v>
       </c>
       <c r="I21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
@@ -2706,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -2715,13 +2692,13 @@
         <v>1</v>
       </c>
       <c r="I22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -2789,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
@@ -2798,13 +2775,13 @@
         <v>1</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" t="b">
         <v>1</v>
@@ -2872,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
@@ -2881,13 +2858,13 @@
         <v>1</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" t="b">
         <v>1</v>
@@ -2955,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
@@ -2964,13 +2941,13 @@
         <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="b">
         <v>1</v>
@@ -3038,7 +3015,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -3047,13 +3024,13 @@
         <v>1</v>
       </c>
       <c r="I26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" t="b">
         <v>1</v>
@@ -3121,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -3130,13 +3107,13 @@
         <v>1</v>
       </c>
       <c r="I27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" t="b">
         <v>1</v>
@@ -3204,7 +3181,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -3213,13 +3190,13 @@
         <v>1</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" t="b">
         <v>1</v>
@@ -3287,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -3296,13 +3273,13 @@
         <v>1</v>
       </c>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" t="b">
         <v>1</v>
@@ -3370,7 +3347,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -3379,13 +3356,13 @@
         <v>1</v>
       </c>
       <c r="I30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" t="b">
         <v>1</v>
@@ -3453,7 +3430,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -3462,13 +3439,13 @@
         <v>1</v>
       </c>
       <c r="I31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" t="b">
         <v>1</v>
@@ -3536,7 +3513,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -3545,13 +3522,13 @@
         <v>1</v>
       </c>
       <c r="I32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" t="b">
         <v>1</v>
@@ -3619,7 +3596,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -3628,13 +3605,13 @@
         <v>1</v>
       </c>
       <c r="I33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" t="b">
         <v>1</v>
@@ -3702,7 +3679,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
@@ -3711,13 +3688,13 @@
         <v>1</v>
       </c>
       <c r="I34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L34" t="b">
         <v>1</v>
@@ -3785,7 +3762,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
@@ -3794,13 +3771,13 @@
         <v>1</v>
       </c>
       <c r="I35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" t="b">
         <v>1</v>
@@ -3868,7 +3845,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -3877,13 +3854,13 @@
         <v>1</v>
       </c>
       <c r="I36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" t="b">
         <v>1</v>
@@ -3951,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -3960,13 +3937,13 @@
         <v>1</v>
       </c>
       <c r="I37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37" t="b">
         <v>1</v>
@@ -4034,7 +4011,7 @@
         <v>1</v>
       </c>
       <c r="F38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -4043,13 +4020,13 @@
         <v>1</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" t="b">
         <v>1</v>
@@ -4117,7 +4094,7 @@
         <v>1</v>
       </c>
       <c r="F39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" t="b">
         <v>1</v>
@@ -4126,13 +4103,13 @@
         <v>1</v>
       </c>
       <c r="I39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" t="b">
         <v>1</v>
@@ -4200,7 +4177,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -4209,13 +4186,13 @@
         <v>1</v>
       </c>
       <c r="I40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" t="b">
         <v>1</v>
@@ -4283,7 +4260,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="b">
         <v>1</v>
@@ -4292,13 +4269,13 @@
         <v>1</v>
       </c>
       <c r="I41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" t="b">
         <v>1</v>
@@ -4366,7 +4343,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -4375,13 +4352,13 @@
         <v>1</v>
       </c>
       <c r="I42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" t="b">
         <v>1</v>
@@ -4449,7 +4426,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
@@ -4458,13 +4435,13 @@
         <v>1</v>
       </c>
       <c r="I43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" t="b">
         <v>1</v>
@@ -4532,7 +4509,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -4541,13 +4518,13 @@
         <v>1</v>
       </c>
       <c r="I44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" t="b">
         <v>1</v>
@@ -4615,7 +4592,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" t="b">
         <v>1</v>
@@ -4624,13 +4601,13 @@
         <v>1</v>
       </c>
       <c r="I45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" t="b">
         <v>1</v>
@@ -4698,7 +4675,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -4707,13 +4684,13 @@
         <v>1</v>
       </c>
       <c r="I46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" t="b">
         <v>1</v>
@@ -4781,7 +4758,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
@@ -4790,13 +4767,13 @@
         <v>1</v>
       </c>
       <c r="I47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" t="b">
         <v>1</v>
@@ -4864,7 +4841,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -4873,13 +4850,13 @@
         <v>1</v>
       </c>
       <c r="I48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" t="b">
         <v>1</v>
@@ -4947,7 +4924,7 @@
         <v>1</v>
       </c>
       <c r="F49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" t="b">
         <v>1</v>
@@ -4956,13 +4933,13 @@
         <v>1</v>
       </c>
       <c r="I49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" t="b">
         <v>1</v>
@@ -5030,7 +5007,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="b">
         <v>1</v>
@@ -5039,13 +5016,13 @@
         <v>1</v>
       </c>
       <c r="I50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" t="b">
         <v>1</v>
@@ -5113,7 +5090,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -5122,13 +5099,13 @@
         <v>1</v>
       </c>
       <c r="I51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" t="b">
         <v>1</v>
@@ -5196,7 +5173,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="b">
         <v>1</v>
@@ -5205,13 +5182,13 @@
         <v>1</v>
       </c>
       <c r="I52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" t="b">
         <v>1</v>
@@ -5279,7 +5256,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" t="b">
         <v>1</v>
@@ -5288,13 +5265,13 @@
         <v>1</v>
       </c>
       <c r="I53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53" t="b">
         <v>1</v>
@@ -5362,7 +5339,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="b">
         <v>1</v>
@@ -5371,13 +5348,13 @@
         <v>1</v>
       </c>
       <c r="I54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54" t="b">
         <v>1</v>
@@ -5445,7 +5422,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" t="b">
         <v>1</v>
@@ -5454,13 +5431,13 @@
         <v>1</v>
       </c>
       <c r="I55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" t="b">
         <v>1</v>
@@ -5528,7 +5505,7 @@
         <v>1</v>
       </c>
       <c r="F56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="b">
         <v>1</v>
@@ -5537,13 +5514,13 @@
         <v>1</v>
       </c>
       <c r="I56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56" t="b">
         <v>1</v>
@@ -5611,7 +5588,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" t="b">
         <v>1</v>
@@ -5620,13 +5597,13 @@
         <v>1</v>
       </c>
       <c r="I57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" t="b">
         <v>1</v>
@@ -5694,7 +5671,7 @@
         <v>1</v>
       </c>
       <c r="F58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" t="b">
         <v>1</v>
@@ -5703,13 +5680,13 @@
         <v>1</v>
       </c>
       <c r="I58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L58" t="b">
         <v>1</v>
@@ -5777,7 +5754,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59" t="b">
         <v>1</v>
@@ -5786,13 +5763,13 @@
         <v>1</v>
       </c>
       <c r="I59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59" t="b">
         <v>1</v>
@@ -5860,7 +5837,7 @@
         <v>1</v>
       </c>
       <c r="F60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" t="b">
         <v>1</v>
@@ -5869,13 +5846,13 @@
         <v>1</v>
       </c>
       <c r="I60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60" t="b">
         <v>1</v>
@@ -5943,7 +5920,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" t="b">
         <v>1</v>
@@ -5952,13 +5929,13 @@
         <v>1</v>
       </c>
       <c r="I61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" t="b">
         <v>1</v>
@@ -6026,7 +6003,7 @@
         <v>1</v>
       </c>
       <c r="F62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" t="b">
         <v>1</v>
@@ -6035,13 +6012,13 @@
         <v>1</v>
       </c>
       <c r="I62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L62" t="b">
         <v>1</v>
@@ -6109,7 +6086,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" t="b">
         <v>1</v>
@@ -6118,13 +6095,13 @@
         <v>1</v>
       </c>
       <c r="I63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L63" t="b">
         <v>1</v>
@@ -6192,7 +6169,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="b">
         <v>1</v>
@@ -6201,13 +6178,13 @@
         <v>1</v>
       </c>
       <c r="I64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64" t="b">
         <v>1</v>
@@ -6275,7 +6252,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" t="b">
         <v>1</v>
@@ -6284,13 +6261,13 @@
         <v>1</v>
       </c>
       <c r="I65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L65" t="b">
         <v>1</v>
@@ -6358,7 +6335,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" t="b">
         <v>1</v>
@@ -6367,13 +6344,13 @@
         <v>1</v>
       </c>
       <c r="I66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L66" t="b">
         <v>1</v>
@@ -6441,7 +6418,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" t="b">
         <v>1</v>
@@ -6450,13 +6427,13 @@
         <v>1</v>
       </c>
       <c r="I67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L67" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
added new variable established_in_waterbody
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E38460-96B4-4E41-83AD-CAB0FAA1F926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF58501-A22F-43DF-86ED-D736154BCF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="111">
   <si>
     <t>Region</t>
   </si>
@@ -362,6 +362,15 @@
   </si>
   <si>
     <t>Pend-d'Oreille River</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Established_in_Waterbody</t>
   </si>
 </sst>
 </file>
@@ -745,7 +754,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +775,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -778,6 +789,9 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -789,6 +803,9 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -800,6 +817,9 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -811,6 +831,9 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="D5" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -822,6 +845,9 @@
       <c r="C6" t="s">
         <v>105</v>
       </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -832,6 +858,9 @@
       </c>
       <c r="C7" t="s">
         <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functionifying the script to facilitate reading
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/john_phelan_gov_bc_ca/Documents/R_projects/ais_prioritization_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{77B2BF77-AD64-468F-B904-DAA1BD147936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BFD36C4-9672-403D-82AD-0F346C1B8411}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB0595F-8A9F-4C2C-8279-FB4D889D6E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="127">
   <si>
     <t>Region</t>
   </si>
@@ -402,6 +402,24 @@
   </si>
   <si>
     <t>Aluminum_Dissolved</t>
+  </si>
+  <si>
+    <t>Watershed</t>
+  </si>
+  <si>
+    <t>Columbia River Watershed</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Smallmouth bass, Goldfish, Pumpkinseed</t>
+  </si>
+  <si>
+    <t>This would run the model for each species in the list for all waterbodies in the chosen watershed THAT HAVE OVERLAPPED WITH SAR (preliminary step); priority ranking is done ACROSS species. Also, have priority columns for MONITORING, DOWNSTREAM EXTENT</t>
+  </si>
+  <si>
+    <t>Fraser River Watershed</t>
   </si>
 </sst>
 </file>
@@ -445,9 +463,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +484,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -786,21 +803,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6445779-2465-4917-922C-4EA6D80CF35A}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,192 +827,226 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>118</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>114</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>96</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>106</v>
       </c>
       <c r="B8" t="s">
         <v>96</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>107</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>115</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>92</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>117</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>112</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>106</v>
       </c>
       <c r="B12" t="s">
         <v>85</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>113</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>79</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>116</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
         <v>104</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>111</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1022,11 +1075,11 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1053,47 +1106,47 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -1107,22 +1160,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9ABB0D-65E2-4F7D-8309-D592BA9BA411}">
   <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48:XFD48"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1208,7 +1261,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1294,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1380,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1466,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1552,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1638,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1724,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1810,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1896,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1982,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2068,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2154,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2240,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2326,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2412,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2498,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2584,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2670,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2756,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -2842,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -2928,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -3014,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3100,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -3186,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -3272,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -3358,7 +3411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -3444,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -3530,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -3616,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -3702,7 +3755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -3788,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -3874,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -3960,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -4046,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -4132,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -4218,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -4304,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -4390,7 +4443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -4476,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -4562,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -4648,7 +4701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -4734,7 +4787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -4820,7 +4873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -4906,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -4992,7 +5045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -5078,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -5164,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -5250,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -5336,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -5422,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -5508,7 +5561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -5594,7 +5647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -5680,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -5766,7 +5819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -5852,7 +5905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -5938,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -6024,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -6110,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>96</v>
       </c>
@@ -6196,7 +6249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>97</v>
       </c>
@@ -6282,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>98</v>
       </c>
@@ -6368,7 +6421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>99</v>
       </c>
@@ -6454,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>100</v>
       </c>
@@ -6540,7 +6593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -6626,7 +6679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>102</v>
       </c>
@@ -6712,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>103</v>
       </c>
@@ -6798,7 +6851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
added northern pike to test
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/john_phelan_gov_bc_ca/Documents/R_projects/ais_prioritization_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB0595F-8A9F-4C2C-8279-FB4D889D6E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{DAB0595F-8A9F-4C2C-8279-FB4D889D6E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F404BC5-6BC1-48BD-9DB4-8975602982C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="127">
   <si>
     <t>Region</t>
   </si>
@@ -484,6 +484,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,23 +807,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6445779-2465-4917-922C-4EA6D80CF35A}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,7 +840,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -850,7 +854,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -864,7 +868,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -878,7 +882,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -892,7 +896,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -906,7 +910,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -920,7 +924,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -934,7 +938,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -948,7 +952,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -962,7 +966,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -976,7 +980,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -990,7 +994,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>124</v>
       </c>
@@ -1035,7 +1039,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>124</v>
       </c>
@@ -1047,6 +1051,17 @@
       </c>
       <c r="E16" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1075,11 +1090,11 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1106,47 +1121,47 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -1165,17 +1180,17 @@
       <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1261,7 +1276,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1347,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1433,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1519,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1605,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1691,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1777,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1863,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1949,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2035,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2121,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2207,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2293,7 +2308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2379,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2465,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2551,7 +2566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2637,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2723,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2809,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -2895,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -2981,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -3067,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3153,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -3239,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -3325,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -3411,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -3497,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -3583,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -3669,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -3755,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -3841,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -3927,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -4013,7 +4028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -4099,7 +4114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -4185,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -4271,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -4357,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -4443,7 +4458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -4529,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -4615,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -4701,7 +4716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -4787,7 +4802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -4873,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -4959,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -5045,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -5131,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -5217,7 +5232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -5303,7 +5318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -5389,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -5475,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -5561,7 +5576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -5647,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -5733,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -5819,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -5905,7 +5920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -5991,7 +6006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -6077,7 +6092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -6163,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>96</v>
       </c>
@@ -6249,7 +6264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>97</v>
       </c>
@@ -6335,7 +6350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>98</v>
       </c>
@@ -6421,7 +6436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>99</v>
       </c>
@@ -6507,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>100</v>
       </c>
@@ -6593,7 +6608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -6679,7 +6694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>102</v>
       </c>
@@ -6765,7 +6780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>103</v>
       </c>
@@ -6851,7 +6866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
moved inputs - don't know if it matters...
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/john_phelan_gov_bc_ca/Documents/R_projects/ais_prioritization_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{DAB0595F-8A9F-4C2C-8279-FB4D889D6E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F404BC5-6BC1-48BD-9DB4-8975602982C6}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{DAB0595F-8A9F-4C2C-8279-FB4D889D6E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60F77DDF-2ED1-4B69-84F9-FDC96FC73109}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="126">
   <si>
     <t>Region</t>
   </si>
@@ -414,9 +414,6 @@
   </si>
   <si>
     <t>Smallmouth bass, Goldfish, Pumpkinseed</t>
-  </si>
-  <si>
-    <t>This would run the model for each species in the list for all waterbodies in the chosen watershed THAT HAVE OVERLAPPED WITH SAR (preliminary step); priority ranking is done ACROSS species. Also, have priority columns for MONITORING, DOWNSTREAM EXTENT</t>
   </si>
   <si>
     <t>Fraser River Watershed</t>
@@ -807,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6445779-2465-4917-922C-4EA6D80CF35A}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,45 +838,46 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>119</v>
-      </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -887,38 +885,38 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>109</v>
@@ -926,13 +924,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>108</v>
@@ -943,27 +941,27 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -974,35 +972,35 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E13" t="s">
         <v>109</v>
@@ -1010,58 +1008,44 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
         <v>104</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>111</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" t="s">
-        <v>123</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1074,7 +1058,7 @@
           <x14:formula1>
             <xm:f>acceptable_values!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A1048576</xm:sqref>
+          <xm:sqref>A1 A2:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
adding option to drop rows with zero SARA overlap
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/john_phelan_gov_bc_ca/Documents/R_projects/ais_prioritization_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{DAB0595F-8A9F-4C2C-8279-FB4D889D6E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60F77DDF-2ED1-4B69-84F9-FDC96FC73109}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C17CDBE-4020-49D8-8512-0F250B6792C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
   <sheets>
-    <sheet name="inputs" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="CNF_model" sheetId="1" r:id="rId1"/>
+    <sheet name="manual_enter_wb" sheetId="4" r:id="rId2"/>
     <sheet name="acceptable_values" sheetId="2" r:id="rId3"/>
     <sheet name="species_predvars" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
   <si>
     <t>Region</t>
   </si>
@@ -413,10 +413,10 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Smallmouth bass, Goldfish, Pumpkinseed</t>
-  </si>
-  <si>
     <t>Fraser River Watershed</t>
+  </si>
+  <si>
+    <t>Smallmouth bass, Goldfish, Pumpkinseed, Largemouth bass, Yellow perch, Asian clam, Northern pike, Common carp, Brown bullhead</t>
   </si>
 </sst>
 </file>
@@ -481,10 +481,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -804,23 +800,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6445779-2465-4917-922C-4EA6D80CF35A}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="63.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,9 +833,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>122</v>
@@ -852,200 +848,18 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
         <v>124</v>
-      </c>
-      <c r="C3" t="s">
-        <v>125</v>
       </c>
       <c r="D3" t="s">
         <v>123</v>
       </c>
       <c r="E3" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1058,7 +872,7 @@
           <x14:formula1>
             <xm:f>acceptable_values!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A1 A2:A1048576</xm:sqref>
+          <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1068,28 +882,228 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A209DA1-EB94-4B98-91E7-1060469146A8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{82CF97C2-EA65-4800-8639-75B403DC8653}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5B68123-4BB9-413C-933C-C3EFB5254545}">
           <x14:formula1>
             <xm:f>acceptable_values!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A4</xm:sqref>
+          <xm:sqref>A1:A14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1105,47 +1119,47 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -1164,17 +1178,17 @@
       <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1260,7 +1274,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1346,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1432,7 +1446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1518,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1604,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1690,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1776,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1862,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1948,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2034,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2120,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2206,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2292,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2378,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2464,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2550,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2636,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2722,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2808,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -2894,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -2980,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -3066,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3152,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -3238,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -3324,7 +3338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -3410,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -3496,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -3582,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -3668,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -3754,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -3840,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -3926,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -4012,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -4098,7 +4112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -4184,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -4270,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -4356,7 +4370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -4442,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -4528,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -4614,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -4700,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -4786,7 +4800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -4872,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -4958,7 +4972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -5044,7 +5058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -5130,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -5216,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -5302,7 +5316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -5388,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -5474,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -5560,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -5646,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -5732,7 +5746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -5818,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -5904,7 +5918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -5990,7 +6004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -6076,7 +6090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -6162,7 +6176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>96</v>
       </c>
@@ -6248,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>97</v>
       </c>
@@ -6334,7 +6348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>98</v>
       </c>
@@ -6420,7 +6434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>99</v>
       </c>
@@ -6506,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>100</v>
       </c>
@@ -6592,7 +6606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -6678,7 +6692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>102</v>
       </c>
@@ -6764,7 +6778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>103</v>
       </c>
@@ -6850,7 +6864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>104</v>
       </c>

</xml_diff>